<commit_message>
Update: Excel sheet updated
</commit_message>
<xml_diff>
--- a/server/uploads/excel_files/UHS_2012.xlsx
+++ b/server/uploads/excel_files/UHS_2012.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My_Work\Websites\Educational_Websites\Prelevels\Code\prelevels\server\questionbank\upload_question_file\question_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hafsa\Desktop\prelevels\server\uploads\excel_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B1FDF27-BB7A-463D-9AFB-746FA66B8CC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DABFE2A-DF15-4160-9D21-5A3A47D4F549}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{C13D1BC6-C0AA-455B-9C56-BEFCA76A008A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{C13D1BC6-C0AA-455B-9C56-BEFCA76A008A}"/>
   </bookViews>
   <sheets>
     <sheet name="2022" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="131">
   <si>
     <t>A</t>
   </si>
@@ -391,9 +391,6 @@
     <t>In a circuit, there is a current of 5 amp which is changed such that the current falls to zero in 0.1 sec. If an average e.m.f. of 200 volts is induced, the self-inductance of the circuit will be:</t>
   </si>
   <si>
-    <t>Why correct answer statement goes here</t>
-  </si>
-  <si>
     <t>Topic</t>
   </si>
   <si>
@@ -418,20 +415,29 @@
     <t>Topic 6</t>
   </si>
   <si>
-    <t>Correct Option</t>
-  </si>
-  <si>
-    <t>Why Correct Option</t>
-  </si>
-  <si>
     <t>Question</t>
+  </si>
+  <si>
+    <t>Question Image</t>
+  </si>
+  <si>
+    <t>Answer</t>
+  </si>
+  <si>
+    <t>Answer Explanation</t>
+  </si>
+  <si>
+    <t>www.images.com</t>
+  </si>
+  <si>
+    <t>Answer explanation goes here</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -443,6 +449,14 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -489,10 +503,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -500,8 +515,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -834,20 +853,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8286FE1B-74C6-4226-BFB0-706777D591E1}">
-  <dimension ref="A1:K19"/>
+  <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3"/>
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="3" width="18.28515625" customWidth="1"/>
     <col min="4" max="5" width="18.42578125" customWidth="1"/>
-    <col min="7" max="7" width="18.28515625" customWidth="1"/>
+    <col min="7" max="8" width="18.28515625" customWidth="1"/>
+    <col min="10" max="10" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="40.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="40.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -867,7 +887,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>126</v>
@@ -876,13 +896,16 @@
         <v>127</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="2" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" ht="81" x14ac:dyDescent="0.25">
+      <c r="L1" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="81" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -904,20 +927,23 @@
       <c r="G2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="I2" s="1" t="s">
-        <v>117</v>
-      </c>
       <c r="J2" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="K2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="K2" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="67.5" x14ac:dyDescent="0.25">
+      <c r="L2" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="54" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
@@ -939,20 +965,23 @@
       <c r="G3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="1" t="s">
-        <v>117</v>
-      </c>
       <c r="J3" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="K3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="K3" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="67.5" x14ac:dyDescent="0.25">
+      <c r="L3" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="54" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>20</v>
       </c>
@@ -974,20 +1003,23 @@
       <c r="G4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H4" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="I4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="I4" s="1" t="s">
-        <v>117</v>
-      </c>
       <c r="J4" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="K4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="K4" s="2" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="L4" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>26</v>
       </c>
@@ -1009,20 +1041,23 @@
       <c r="G5" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="H5" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="I5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I5" s="1" t="s">
-        <v>117</v>
-      </c>
       <c r="J5" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="K5" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="K5" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="148.5" x14ac:dyDescent="0.25">
+      <c r="L5" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="148.5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>33</v>
       </c>
@@ -1044,20 +1079,23 @@
       <c r="G6" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="H6" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="I6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="I6" s="1" t="s">
-        <v>117</v>
-      </c>
       <c r="J6" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="K6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="K6" s="2" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="67.5" x14ac:dyDescent="0.25">
+      <c r="L6" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="54" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>39</v>
       </c>
@@ -1079,20 +1117,23 @@
       <c r="G7" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="H7" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="I7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="I7" s="1" t="s">
-        <v>117</v>
-      </c>
       <c r="J7" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="K7" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="K7" s="2" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="67.5" x14ac:dyDescent="0.25">
+      <c r="L7" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="54" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>44</v>
       </c>
@@ -1114,20 +1155,23 @@
       <c r="G8" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="H8" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="I8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I8" s="1" t="s">
-        <v>117</v>
-      </c>
       <c r="J8" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="K8" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="K8" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="67.5" x14ac:dyDescent="0.25">
+      <c r="L8" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="54" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>51</v>
       </c>
@@ -1149,20 +1193,23 @@
       <c r="G9" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="H9" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="I9" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="I9" s="1" t="s">
-        <v>117</v>
-      </c>
       <c r="J9" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="K9" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="K9" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" ht="67.5" x14ac:dyDescent="0.25">
+      <c r="L9" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="54" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>58</v>
       </c>
@@ -1184,20 +1231,23 @@
       <c r="G10" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="H10" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="I10" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="I10" s="1" t="s">
-        <v>117</v>
-      </c>
       <c r="J10" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="K10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="K10" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" ht="67.5" x14ac:dyDescent="0.25">
+      <c r="L10" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>64</v>
       </c>
@@ -1219,20 +1269,23 @@
       <c r="G11" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="H11" s="1" t="s">
+      <c r="H11" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="I11" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="I11" s="1" t="s">
-        <v>117</v>
-      </c>
       <c r="J11" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="K11" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="K11" s="2" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" ht="67.5" x14ac:dyDescent="0.25">
+      <c r="L11" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>70</v>
       </c>
@@ -1254,20 +1307,23 @@
       <c r="G12" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="H12" s="1" t="s">
+      <c r="H12" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="I12" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="I12" s="1" t="s">
-        <v>117</v>
-      </c>
       <c r="J12" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="K12" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="K12" s="2" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="67.5" x14ac:dyDescent="0.25">
+      <c r="L12" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="54" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>75</v>
       </c>
@@ -1289,20 +1345,23 @@
       <c r="G13" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="H13" s="1" t="s">
+      <c r="H13" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="I13" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="I13" s="1" t="s">
-        <v>117</v>
-      </c>
       <c r="J13" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="K13" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="K13" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" ht="67.5" x14ac:dyDescent="0.25">
+      <c r="L13" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>81</v>
       </c>
@@ -1324,20 +1383,23 @@
       <c r="G14" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="H14" s="1" t="s">
+      <c r="H14" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="I14" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="I14" s="1" t="s">
-        <v>117</v>
-      </c>
       <c r="J14" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="K14" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="K14" s="2" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" ht="67.5" x14ac:dyDescent="0.25">
+      <c r="L14" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="54" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>87</v>
       </c>
@@ -1359,20 +1421,23 @@
       <c r="G15" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="H15" s="1" t="s">
+      <c r="H15" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="I15" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="I15" s="1" t="s">
-        <v>117</v>
-      </c>
       <c r="J15" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="K15" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="K15" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" ht="108" x14ac:dyDescent="0.25">
+      <c r="L15" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="108" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>93</v>
       </c>
@@ -1394,20 +1459,23 @@
       <c r="G16" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="H16" s="1" t="s">
+      <c r="H16" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="I16" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="I16" s="1" t="s">
-        <v>117</v>
-      </c>
       <c r="J16" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="K16" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="K16" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" ht="135" x14ac:dyDescent="0.25">
+      <c r="L16" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="135" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>99</v>
       </c>
@@ -1429,20 +1497,23 @@
       <c r="G17" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="H17" s="1" t="s">
+      <c r="H17" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="I17" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="I17" s="1" t="s">
-        <v>117</v>
-      </c>
       <c r="J17" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="K17" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="K17" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" ht="67.5" x14ac:dyDescent="0.25">
+      <c r="L17" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>105</v>
       </c>
@@ -1464,20 +1535,23 @@
       <c r="G18" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="H18" s="1" t="s">
+      <c r="H18" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="I18" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I18" s="1" t="s">
-        <v>117</v>
-      </c>
       <c r="J18" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="K18" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="K18" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" ht="121.5" x14ac:dyDescent="0.25">
+      <c r="L18" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="121.5" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>111</v>
       </c>
@@ -1499,25 +1573,32 @@
       <c r="G19" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="H19" s="1" t="s">
+      <c r="H19" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="I19" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="I19" s="1" t="s">
-        <v>117</v>
-      </c>
       <c r="J19" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="K19" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="K19" s="2" t="s">
-        <v>119</v>
+      <c r="L19" s="2" t="s">
+        <v>118</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="J2:J19" xr:uid="{D0890A79-EE04-4AE0-B415-163B46E22875}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="K2:K19" xr:uid="{D0890A79-EE04-4AE0-B415-163B46E22875}">
       <formula1>"Biology,Chemistry,Physics,English,Logical Reasoning"</formula1>
     </dataValidation>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="H2" r:id="rId1" xr:uid="{9F30AD61-0B72-4247-BD31-3FC640E1BA1B}"/>
+    <hyperlink ref="H3:H19" r:id="rId2" display="www.images.com" xr:uid="{7FAA42F6-307E-4C91-B76A-135B8B0DB237}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>